<commit_message>
New Version of KWKG with variable full load hour calculation
</commit_message>
<xml_diff>
--- a/raw_inputs/devices.xlsx
+++ b/raw_inputs/devices.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Subsidy-Optimization\raw_inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04_Subsidy-Optimization\raw_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15" yWindow="30" windowWidth="14415" windowHeight="13380" activeTab="8"/>
+    <workbookView xWindow="15" yWindow="30" windowWidth="14415" windowHeight="13380" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="boiler" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="117">
   <si>
     <t>Number</t>
   </si>
@@ -375,6 +375,18 @@
   </si>
   <si>
     <t>dT_max in K</t>
+  </si>
+  <si>
+    <t>Preise für Batteriesysteme in Anhlehnung an den Jahresbericht 2017 für das Batteriespeichermonitoring</t>
+  </si>
+  <si>
+    <t>1.000 €/kWh für den größten Speicher</t>
+  </si>
+  <si>
+    <t>Die anderen bewegen sich dazwischen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.700 €/kWh für den kleinsten Speicher </t>
   </si>
 </sst>
 </file>
@@ -386,7 +398,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,6 +417,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -440,7 +458,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -463,6 +481,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1095,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,11 +1165,12 @@
         <v>1</v>
       </c>
       <c r="B2" s="10">
-        <v>3823.5</v>
+        <f>6.4*1700</f>
+        <v>10880</v>
       </c>
       <c r="C2" s="11">
         <f>B2*0.01</f>
-        <v>38.234999999999999</v>
+        <v>108.8</v>
       </c>
       <c r="D2" s="4">
         <v>15</v>
@@ -1170,18 +1190,21 @@
       <c r="I2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="5"/>
+      <c r="J2" s="20" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="10">
-        <v>4215</v>
+        <f>8*1500</f>
+        <v>12000</v>
       </c>
       <c r="C3" s="11">
         <f t="shared" ref="C3:C6" si="0">B3*0.01</f>
-        <v>42.15</v>
+        <v>120</v>
       </c>
       <c r="D3" s="4">
         <v>15</v>
@@ -1201,18 +1224,21 @@
       <c r="I3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="5"/>
+      <c r="J3" s="5" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="10">
-        <v>5009.2500000000009</v>
+        <f>11*1300</f>
+        <v>14300</v>
       </c>
       <c r="C4" s="11">
         <f t="shared" si="0"/>
-        <v>50.092500000000008</v>
+        <v>143</v>
       </c>
       <c r="D4" s="4">
         <v>15</v>
@@ -1232,18 +1258,21 @@
       <c r="I4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="5"/>
+      <c r="J4" s="5" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="10">
-        <v>5984.2500000000009</v>
+        <f>16*1100</f>
+        <v>17600</v>
       </c>
       <c r="C5" s="11">
         <f t="shared" si="0"/>
-        <v>59.842500000000008</v>
+        <v>176</v>
       </c>
       <c r="D5" s="4">
         <v>15</v>
@@ -1263,18 +1292,21 @@
       <c r="I5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J5" s="5"/>
+      <c r="J5" s="5" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="10">
-        <v>6846.75</v>
+        <f>22*1000</f>
+        <v>22000</v>
       </c>
       <c r="C6" s="11">
         <f t="shared" si="0"/>
-        <v>68.467500000000001</v>
+        <v>220</v>
       </c>
       <c r="D6" s="4">
         <v>15</v>
@@ -1378,6 +1410,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3648,7 +3681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Remove all subsidy programs Add old oil and gas boiler
</commit_message>
<xml_diff>
--- a/raw_inputs/devices.xlsx
+++ b/raw_inputs/devices.xlsx
@@ -5,26 +5,30 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Forschung\EBC0324_BMWi_BF2016_tos\Students\srm-jba\Programme\Subsidy-Optimization-Vent\raw_inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\10_Git\Subsidy-Optimization\raw_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15" yWindow="30" windowWidth="14415" windowHeight="13380" activeTab="9"/>
+    <workbookView xWindow="20" yWindow="30" windowWidth="14420" windowHeight="13380" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="boiler" sheetId="4" r:id="rId1"/>
-    <sheet name="pellet" sheetId="12" r:id="rId2"/>
-    <sheet name="chp" sheetId="3" r:id="rId3"/>
-    <sheet name="eh" sheetId="1" r:id="rId4"/>
-    <sheet name="hp_air" sheetId="2" r:id="rId5"/>
-    <sheet name="hp_geo" sheetId="11" r:id="rId6"/>
-    <sheet name="pv" sheetId="6" r:id="rId7"/>
-    <sheet name="stc" sheetId="7" r:id="rId8"/>
-    <sheet name="tes" sheetId="8" r:id="rId9"/>
-    <sheet name="bat" sheetId="9" r:id="rId10"/>
+    <sheet name="boiler_gas_old" sheetId="15" r:id="rId1"/>
+    <sheet name="boiler_oil_old" sheetId="14" r:id="rId2"/>
+    <sheet name="boiler" sheetId="4" r:id="rId3"/>
+    <sheet name="pellet" sheetId="12" r:id="rId4"/>
+    <sheet name="chp" sheetId="3" r:id="rId5"/>
+    <sheet name="eh" sheetId="1" r:id="rId6"/>
+    <sheet name="hp_air" sheetId="2" r:id="rId7"/>
+    <sheet name="hp_geo" sheetId="11" r:id="rId8"/>
+    <sheet name="pv" sheetId="6" r:id="rId9"/>
+    <sheet name="stc" sheetId="7" r:id="rId10"/>
+    <sheet name="tes" sheetId="8" r:id="rId11"/>
+    <sheet name="bat" sheetId="9" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">boiler!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">boiler!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">boiler_gas_old!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">boiler_oil_old!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="118">
   <si>
     <t>Number</t>
   </si>
@@ -387,6 +391,9 @@
   </si>
   <si>
     <t xml:space="preserve">1.700 €/kWh für den kleinsten Speicher </t>
+  </si>
+  <si>
+    <t>no investment, eta estimated</t>
   </si>
 </sst>
 </file>
@@ -763,346 +770,309 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection sqref="A1:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.26953125" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="10.90625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
-        <v>106</v>
-      </c>
-      <c r="K1" t="s">
-        <v>107</v>
-      </c>
-      <c r="L1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
         <v>15</v>
       </c>
       <c r="C2" s="2">
         <v>0.3</v>
       </c>
       <c r="D2" s="18">
-        <f>$J$2+B2*$K$2+B2^2*$L$2</f>
-        <v>4126.54</v>
+        <v>0</v>
       </c>
       <c r="E2" s="2">
-        <f t="shared" ref="E2:E11" si="0">D2*0.025</f>
         <v>103.1635</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="6">
         <v>20</v>
       </c>
       <c r="G2" s="2">
-        <v>0.93</v>
+        <v>0.85</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2">
-        <v>3142.9</v>
-      </c>
-      <c r="K2">
-        <v>66.44</v>
-      </c>
-      <c r="L2">
-        <v>-5.7599999999999998E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>22</v>
       </c>
       <c r="C3" s="2">
         <v>0.3</v>
       </c>
       <c r="D3" s="18">
-        <f t="shared" ref="D3:D11" si="1">$J$2+B3*$K$2+B3^2*$L$2</f>
-        <v>4576.7016000000003</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" si="0"/>
         <v>114.41754000000002</v>
       </c>
       <c r="F3" s="6">
         <v>20</v>
       </c>
       <c r="G3" s="2">
-        <v>0.93</v>
+        <v>0.85</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
         <v>30</v>
       </c>
       <c r="C4" s="2">
         <v>0.3</v>
       </c>
       <c r="D4" s="18">
-        <f t="shared" si="1"/>
-        <v>5084.26</v>
+        <v>0</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="0"/>
         <v>127.10650000000001</v>
       </c>
       <c r="F4" s="6">
         <v>20</v>
       </c>
       <c r="G4" s="2">
-        <v>0.93</v>
+        <v>0.85</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="6">
         <v>40</v>
       </c>
       <c r="C5" s="2">
         <v>0.3</v>
       </c>
       <c r="D5" s="18">
-        <f t="shared" si="1"/>
-        <v>5708.34</v>
+        <v>0</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="0"/>
         <v>142.70850000000002</v>
       </c>
       <c r="F5" s="6">
         <v>20</v>
       </c>
       <c r="G5" s="2">
-        <v>0.93</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
+        <v>0.85</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="6">
         <v>50</v>
       </c>
       <c r="C6" s="2">
         <v>0.3</v>
       </c>
       <c r="D6" s="18">
-        <f t="shared" si="1"/>
-        <v>6320.9</v>
+        <v>0</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="0"/>
         <v>158.02250000000001</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="6">
         <v>20</v>
       </c>
       <c r="G6" s="2">
-        <v>0.93</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7">
+        <v>0.85</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="6">
         <v>120</v>
       </c>
       <c r="C7" s="2">
         <v>0.25</v>
       </c>
       <c r="D7" s="18">
-        <f t="shared" si="1"/>
-        <v>10286.259999999998</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="0"/>
         <v>257.15649999999999</v>
       </c>
       <c r="F7" s="6">
         <v>20</v>
       </c>
       <c r="G7" s="2">
-        <v>0.97</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8">
+        <v>0.85</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="6">
         <v>160</v>
       </c>
       <c r="C8" s="2">
         <v>0.25</v>
       </c>
       <c r="D8" s="18">
-        <f t="shared" si="1"/>
-        <v>12298.74</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="0"/>
         <v>307.46850000000001</v>
       </c>
       <c r="F8" s="6">
         <v>20</v>
       </c>
       <c r="G8" s="2">
-        <v>0.97</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9">
+        <v>0.85</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="6">
         <v>200</v>
       </c>
       <c r="C9" s="2">
         <v>0.25</v>
       </c>
       <c r="D9" s="18">
-        <f t="shared" si="1"/>
-        <v>14126.900000000001</v>
+        <v>0</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="0"/>
         <v>353.17250000000007</v>
       </c>
       <c r="F9" s="6">
         <v>20</v>
       </c>
       <c r="G9" s="2">
-        <v>0.97</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10">
+        <v>0.85</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="6">
         <v>240</v>
       </c>
       <c r="C10" s="2">
         <v>0.25</v>
       </c>
       <c r="D10" s="18">
-        <f t="shared" si="1"/>
-        <v>15770.74</v>
+        <v>0</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="0"/>
         <v>394.26850000000002</v>
       </c>
       <c r="F10" s="6">
         <v>20</v>
       </c>
       <c r="G10" s="2">
-        <v>0.97</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11">
+        <v>0.85</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="6">
         <v>280</v>
       </c>
       <c r="C11" s="2">
         <v>0.25</v>
       </c>
       <c r="D11" s="18">
-        <f t="shared" si="1"/>
-        <v>17230.260000000002</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="0"/>
         <v>430.75650000000007</v>
       </c>
       <c r="F11" s="6">
         <v>20</v>
       </c>
       <c r="G11" s="2">
-        <v>0.97</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>62</v>
+        <v>0.85</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1112,26 +1082,555 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>843</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2" si="0">B2*0.015</f>
+        <v>12.645</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="G2">
+        <v>3.235E-3</v>
+      </c>
+      <c r="H2" s="19">
+        <v>1.17E-5</v>
+      </c>
+      <c r="I2" s="12">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="2"/>
+      <c r="I3" s="12"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="2"/>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="2"/>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="2"/>
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I10" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7265625" customWidth="1"/>
+    <col min="9" max="9" width="11.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>585</v>
+      </c>
+      <c r="C2">
+        <v>11.7</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F2">
+        <v>0.12</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="6">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>735</v>
+      </c>
+      <c r="C3">
+        <v>14.7</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1075</v>
+      </c>
+      <c r="C4">
+        <v>21.5</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>3.23</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="6">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1580</v>
+      </c>
+      <c r="C5">
+        <v>31.6</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>3.89</v>
+      </c>
+      <c r="F5">
+        <v>1.5</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="6">
+        <v>30</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1710</v>
+      </c>
+      <c r="C6">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>5.4</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6">
+        <v>30</v>
+      </c>
+      <c r="J6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1835</v>
+      </c>
+      <c r="C7">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>5.8</v>
+      </c>
+      <c r="F7">
+        <v>2.5</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="6">
+        <v>30</v>
+      </c>
+      <c r="J7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2080</v>
+      </c>
+      <c r="C8">
+        <v>41.6</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>6.1</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6">
+        <v>30</v>
+      </c>
+      <c r="J8" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2955</v>
+      </c>
+      <c r="C9">
+        <v>59.1</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6">
+        <v>30</v>
+      </c>
+      <c r="J9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3415</v>
+      </c>
+      <c r="C10">
+        <v>68.3</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>11.2</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="6">
+        <v>30</v>
+      </c>
+      <c r="J10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>5130</v>
+      </c>
+      <c r="C11">
+        <v>102.6</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>18.3</v>
+      </c>
+      <c r="F11">
+        <v>7.5</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" s="6">
+        <v>30</v>
+      </c>
+      <c r="J11" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="53.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="53.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1194,7 +1693,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1228,7 +1727,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1262,7 +1761,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1296,7 +1795,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1328,84 +1827,84 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J33" s="2"/>
     </row>
   </sheetData>
@@ -1416,25 +1915,686 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.26953125" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="10.90625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D2" s="18">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>103.1635</v>
+      </c>
+      <c r="F2" s="6">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D3" s="18">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>114.41754000000002</v>
+      </c>
+      <c r="F3" s="6">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="18">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>127.10650000000001</v>
+      </c>
+      <c r="F4" s="6">
+        <v>20</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>40</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>142.70850000000002</v>
+      </c>
+      <c r="F5" s="6">
+        <v>20</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>50</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>158.02250000000001</v>
+      </c>
+      <c r="F6" s="6">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>120</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D7" s="18">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>257.15649999999999</v>
+      </c>
+      <c r="F7" s="6">
+        <v>20</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6">
+        <v>160</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D8" s="18">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>307.46850000000001</v>
+      </c>
+      <c r="F8" s="6">
+        <v>20</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6">
+        <v>200</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D9" s="18">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>353.17250000000007</v>
+      </c>
+      <c r="F9" s="6">
+        <v>20</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6">
+        <v>240</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D10" s="18">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>394.26850000000002</v>
+      </c>
+      <c r="F10" s="6">
+        <v>20</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
+        <v>280</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D11" s="18">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>430.75650000000007</v>
+      </c>
+      <c r="F11" s="6">
+        <v>20</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D2" s="18">
+        <f>$J$2+B2*$K$2+B2^2*$L$2</f>
+        <v>4126.54</v>
+      </c>
+      <c r="E2" s="2">
+        <f t="shared" ref="E2:E11" si="0">D2*0.025</f>
+        <v>103.1635</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.93</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2">
+        <v>3142.9</v>
+      </c>
+      <c r="K2">
+        <v>66.44</v>
+      </c>
+      <c r="L2">
+        <v>-5.7599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D3" s="18">
+        <f t="shared" ref="D3:D11" si="1">$J$2+B3*$K$2+B3^2*$L$2</f>
+        <v>4576.7016000000003</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" si="0"/>
+        <v>114.41754000000002</v>
+      </c>
+      <c r="F3" s="6">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.93</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="18">
+        <f t="shared" si="1"/>
+        <v>5084.26</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>127.10650000000001</v>
+      </c>
+      <c r="F4" s="6">
+        <v>20</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.93</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D5" s="18">
+        <f t="shared" si="1"/>
+        <v>5708.34</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>142.70850000000002</v>
+      </c>
+      <c r="F5" s="6">
+        <v>20</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.93</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D6" s="18">
+        <f t="shared" si="1"/>
+        <v>6320.9</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>158.02250000000001</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.93</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>120</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D7" s="18">
+        <f t="shared" si="1"/>
+        <v>10286.259999999998</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>257.15649999999999</v>
+      </c>
+      <c r="F7" s="6">
+        <v>20</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>160</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D8" s="18">
+        <f t="shared" si="1"/>
+        <v>12298.74</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>307.46850000000001</v>
+      </c>
+      <c r="F8" s="6">
+        <v>20</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>200</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D9" s="18">
+        <f t="shared" si="1"/>
+        <v>14126.900000000001</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>353.17250000000007</v>
+      </c>
+      <c r="F9" s="6">
+        <v>20</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>240</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D10" s="18">
+        <f t="shared" si="1"/>
+        <v>15770.74</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>394.26850000000002</v>
+      </c>
+      <c r="F10" s="6">
+        <v>20</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>280</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D11" s="18">
+        <f t="shared" si="1"/>
+        <v>17230.260000000002</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>430.75650000000007</v>
+      </c>
+      <c r="F11" s="6">
+        <v>20</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="63.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="63.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>110</v>
       </c>
@@ -1469,7 +2629,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1506,7 +2666,7 @@
         <v>-0.3639</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1534,7 +2694,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1562,7 +2722,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1590,7 +2750,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1618,7 +2778,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1646,7 +2806,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1674,7 +2834,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1702,7 +2862,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1730,7 +2890,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -1758,7 +2918,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="2"/>
@@ -1768,7 +2928,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="2"/>
@@ -1783,7 +2943,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
@@ -1791,20 +2951,20 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>110</v>
       </c>
@@ -1839,7 +2999,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1876,7 +3036,7 @@
         <v>500.9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1908,7 +3068,7 @@
       </c>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1939,7 +3099,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1970,7 +3130,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2002,7 +3162,7 @@
       </c>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2033,7 +3193,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2064,7 +3224,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2095,7 +3255,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2126,68 +3286,68 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D26" s="2"/>
     </row>
   </sheetData>
@@ -2195,7 +3355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -2203,19 +3363,19 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>110</v>
       </c>
@@ -2238,7 +3398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2262,7 +3422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2291,7 +3451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S11"/>
   <sheetViews>
@@ -2299,27 +3459,27 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>110</v>
       </c>
@@ -2375,7 +3535,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -2433,7 +3593,7 @@
         <v>881.48</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -2485,7 +3645,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -2537,7 +3697,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -2589,7 +3749,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -2641,7 +3801,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -2693,7 +3853,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -2745,7 +3905,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -2797,7 +3957,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -2807,7 +3967,7 @@
       <c r="G10" s="6"/>
       <c r="P10" s="7"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="6"/>
     </row>
   </sheetData>
@@ -2815,7 +3975,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S15"/>
   <sheetViews>
@@ -2823,27 +3983,27 @@
       <selection activeCell="G1" sqref="G1:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>110</v>
       </c>
@@ -2899,7 +4059,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -2957,7 +4117,7 @@
         <v>614.80999999999995</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -3009,7 +4169,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -3061,7 +4221,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -3113,7 +4273,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -3165,7 +4325,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -3217,7 +4377,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -3269,7 +4429,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -3321,7 +4481,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -3373,13 +4533,13 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="F11" s="17"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="F14" s="17"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="H15" s="17"/>
     </row>
   </sheetData>
@@ -3387,7 +4547,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
@@ -3395,21 +4555,21 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" customWidth="1"/>
+    <col min="9" max="9" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3441,7 +4601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3474,7 +4634,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -3507,579 +4667,50 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
       <c r="F13" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>843</v>
-      </c>
-      <c r="C2">
-        <f t="shared" ref="C2" si="0">B2*0.015</f>
-        <v>12.645</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>0.80400000000000005</v>
-      </c>
-      <c r="G2">
-        <v>3.235E-3</v>
-      </c>
-      <c r="H2" s="19">
-        <v>1.17E-5</v>
-      </c>
-      <c r="I2" s="12">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="I3" s="12"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="I4" s="12"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I10" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>585</v>
-      </c>
-      <c r="C2">
-        <v>11.7</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-      <c r="E2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F2">
-        <v>0.12</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="6">
-        <v>30</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>735</v>
-      </c>
-      <c r="C3">
-        <v>14.7</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="E3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F3">
-        <v>0.5</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="6">
-        <v>30</v>
-      </c>
-      <c r="J3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1075</v>
-      </c>
-      <c r="C4">
-        <v>21.5</v>
-      </c>
-      <c r="D4">
-        <v>20</v>
-      </c>
-      <c r="E4">
-        <v>3.23</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="6">
-        <v>30</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1580</v>
-      </c>
-      <c r="C5">
-        <v>31.6</v>
-      </c>
-      <c r="D5">
-        <v>20</v>
-      </c>
-      <c r="E5">
-        <v>3.89</v>
-      </c>
-      <c r="F5">
-        <v>1.5</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="6">
-        <v>30</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1710</v>
-      </c>
-      <c r="C6">
-        <v>34.200000000000003</v>
-      </c>
-      <c r="D6">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <v>5.4</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6" s="6">
-        <v>30</v>
-      </c>
-      <c r="J6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>1835</v>
-      </c>
-      <c r="C7">
-        <v>36.700000000000003</v>
-      </c>
-      <c r="D7">
-        <v>20</v>
-      </c>
-      <c r="E7">
-        <v>5.8</v>
-      </c>
-      <c r="F7">
-        <v>2.5</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7" s="6">
-        <v>30</v>
-      </c>
-      <c r="J7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>2080</v>
-      </c>
-      <c r="C8">
-        <v>41.6</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-      <c r="E8">
-        <v>6.1</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8" s="6">
-        <v>30</v>
-      </c>
-      <c r="J8" t="s">
-        <v>43</v>
-      </c>
-      <c r="K8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>2955</v>
-      </c>
-      <c r="C9">
-        <v>59.1</v>
-      </c>
-      <c r="D9">
-        <v>20</v>
-      </c>
-      <c r="E9">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="F9">
-        <v>4</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9" s="6">
-        <v>30</v>
-      </c>
-      <c r="J9" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>3415</v>
-      </c>
-      <c r="C10">
-        <v>68.3</v>
-      </c>
-      <c r="D10">
-        <v>20</v>
-      </c>
-      <c r="E10">
-        <v>11.2</v>
-      </c>
-      <c r="F10">
-        <v>5</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10" s="6">
-        <v>30</v>
-      </c>
-      <c r="J10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>5130</v>
-      </c>
-      <c r="C11">
-        <v>102.6</v>
-      </c>
-      <c r="D11">
-        <v>20</v>
-      </c>
-      <c r="E11">
-        <v>18.3</v>
-      </c>
-      <c r="F11">
-        <v>7.5</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11" s="6">
-        <v>30</v>
-      </c>
-      <c r="J11" t="s">
-        <v>46</v>
-      </c>
-      <c r="K11" t="s">
-        <v>42</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>